<commit_message>
Versión final con ajustes en las referecias a mi repositorio de Github
</commit_message>
<xml_diff>
--- a/UnitTest-ProyectoClub.xlsx
+++ b/UnitTest-ProyectoClub.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agust\Desktop\proyectoFinalCoder\EntregaFinalCoder\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agust\Desktop\EntregaFinalCoder\EntregaFinalCoder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2932F79D-A65E-46A6-8DDB-C914D58993DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9E8E659-5910-4771-8EA9-8E4913B18E88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="39">
   <si>
     <t>Probado por:</t>
   </si>
@@ -115,6 +115,33 @@
   </si>
   <si>
     <t>Luego de realizar el Login se habilitan las opciones de CRUD para cada modelo y al realizar el Logout se deshabilitan</t>
+  </si>
+  <si>
+    <t>Se realiza el proceso de CRUD para un nuevo elemento en 'Plantel'</t>
+  </si>
+  <si>
+    <t>Se busca poder Crear, Leer, Actualizar y Borrar un elemento para 'Plantel'</t>
+  </si>
+  <si>
+    <t>Se llevan a cabo las acciones buscadas para un nuevo elemento en 'Plantel', se creó un nuevo elemento, se lo leyó, se lo editó y se lo borro</t>
+  </si>
+  <si>
+    <t>Eliminar us usuario desde el perfil de administrador</t>
+  </si>
+  <si>
+    <t>Se desea borrar un usuario accediendo como administrador en la ruta '/admin/'</t>
+  </si>
+  <si>
+    <t>Se borra un usuario previamente creado</t>
+  </si>
+  <si>
+    <t>Revisar la restricción para consultar, editar o borrar elementos cargados</t>
+  </si>
+  <si>
+    <t>Sin estar legueado no se debería poder acceder a la vista que permite realizar las funciones detalladas</t>
+  </si>
+  <si>
+    <t>Si no se encuentra loguado no se permite acceder a la vista que permite consultar, editar o borrar los valores cargados</t>
   </si>
 </sst>
 </file>
@@ -218,20 +245,8 @@
   </cellStyleXfs>
   <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -245,6 +260,18 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -535,10 +562,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:G12"/>
+  <dimension ref="B3:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8:G8"/>
+      <selection activeCell="G13" sqref="G13:G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -546,170 +573,230 @@
     <col min="2" max="2" width="22.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.7109375" customWidth="1"/>
     <col min="4" max="4" width="36.5703125" customWidth="1"/>
-    <col min="5" max="5" width="31.28515625" customWidth="1"/>
-    <col min="6" max="6" width="30.7109375" customWidth="1"/>
+    <col min="5" max="5" width="35.85546875" customWidth="1"/>
+    <col min="6" max="6" width="41.85546875" customWidth="1"/>
     <col min="7" max="7" width="23.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="10" t="s">
+      <c r="D3" s="11"/>
+      <c r="E3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="G3" s="1"/>
+      <c r="G3" s="11"/>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="11">
         <v>1</v>
       </c>
-      <c r="D4" s="1"/>
-      <c r="E4" s="10" t="s">
+      <c r="D4" s="11"/>
+      <c r="E4" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="G4" s="1"/>
+      <c r="G4" s="11"/>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="1"/>
-      <c r="E5" s="10" t="s">
+      <c r="D5" s="11"/>
+      <c r="E5" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="G5" s="1"/>
+      <c r="G5" s="11"/>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="1"/>
-      <c r="E6" s="10" t="s">
+      <c r="D6" s="11"/>
+      <c r="E6" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F6" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="G6" s="1"/>
+      <c r="G6" s="11"/>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B7" s="4"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="6"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="10"/>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="D8" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="11" t="s">
+      <c r="E8" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="11" t="s">
+      <c r="F8" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G8" s="11" t="s">
+      <c r="G8" s="7" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="9" spans="2:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="B9" s="3">
+      <c r="B9" s="2">
         <v>1</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C9" s="3">
         <v>44207</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="E9" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F9" s="8" t="s">
+      <c r="F9" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="G9" s="9" t="s">
+      <c r="G9" s="5" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="10" spans="2:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="B10" s="3">
+      <c r="B10" s="2">
         <v>2</v>
       </c>
-      <c r="C10" s="7">
+      <c r="C10" s="3">
         <v>44207</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E10" s="8" t="s">
+      <c r="E10" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F10" s="8" t="s">
+      <c r="F10" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="G10" s="9" t="s">
+      <c r="G10" s="5" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="11" spans="2:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="B11" s="3">
+      <c r="B11" s="2">
         <v>3</v>
       </c>
-      <c r="C11" s="7">
+      <c r="C11" s="3">
         <v>44207</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D11" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E11" s="8" t="s">
+      <c r="E11" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="F11" s="8" t="s">
+      <c r="F11" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="G11" s="9" t="s">
+      <c r="G11" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B12" s="3"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="2"/>
+    <row r="12" spans="2:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="B12" s="2">
+        <v>4</v>
+      </c>
+      <c r="C12" s="3">
+        <v>44573</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="B13" s="2">
+        <v>5</v>
+      </c>
+      <c r="C13" s="3">
+        <v>44573</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="B14" s="2">
+        <v>6</v>
+      </c>
+      <c r="C14" s="3">
+        <v>44573</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="2"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -723,7 +810,7 @@
     <mergeCell ref="F5:G5"/>
     <mergeCell ref="F6:G6"/>
   </mergeCells>
-  <conditionalFormatting sqref="B9:G9 B10:C11 G10:G11">
+  <conditionalFormatting sqref="B9:G9 B10:C11 G10:G14">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"Sí"</formula>
     </cfRule>

</xml_diff>